<commit_message>
export piecewiseyieldcurve functions to excel (183/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/PiecewiseYieldCurve.xlsx
+++ b/UnitTests/Tests/PiecewiseYieldCurve.xlsx
@@ -66,10 +66,10 @@
     <t>qlPiecewiseYieldCurveJumpDates</t>
   </si>
   <si>
-    <t>pwyc01#0044</t>
-  </si>
-  <si>
-    <t>pwyc02#0049</t>
+    <t>pwyc01#0000</t>
+  </si>
+  <si>
+    <t>pwyc02#0000</t>
   </si>
 </sst>
 </file>
@@ -482,11 +482,11 @@
       </c>
       <c r="E3" t="str">
         <f>_xll.qlPiecewiseYieldCurve("pwyc01",0,"target",G3:G5,"Actual/360",H3:H5,I3:I5,0.000000000001,"Discount","LogLinear")</f>
-        <v>pwyc01#0044</v>
+        <v>pwyc01#0000</v>
       </c>
       <c r="G3" t="str">
         <f>_xll.qlFraRateHelper(,1,"1d",J3,"maturitydate")</f>
-        <v>obj_00001#0011</v>
+        <v>obj_00002#0000</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -496,7 +496,7 @@
       </c>
       <c r="J3" t="str">
         <f>_xll.qlIborIndex(,"euribor","1d",2,"eur","target","modified following",TRUE,"actual/360")</f>
-        <v>obj_00000#0008</v>
+        <v>obj_00000#0000</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -512,11 +512,11 @@
       </c>
       <c r="E4" t="str">
         <f>_xll.qlPiecewiseYieldCurveMixedInterpolation("pwyc02",0,"target",G3:G5,"actual/360",H3:H5,I3:I5,0.000000000001,"discount","loglinear","shareranges",0)</f>
-        <v>pwyc02#0049</v>
+        <v>pwyc02#0000</v>
       </c>
       <c r="G4" t="str">
         <f>_xll.qlFraRateHelper(,1,"2d",J3,"maturitydate")</f>
-        <v>obj_00002#0002</v>
+        <v>obj_00001#0000</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -542,7 +542,7 @@
       </c>
       <c r="G5" t="str">
         <f>_xll.qlFraRateHelper(,1,"3d",J3,"maturitydate")</f>
-        <v>obj_00003#0002</v>
+        <v>obj_00003#0000</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -556,7 +556,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="4">
-        <v>42675</v>
+        <v>42676</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="3" t="str">
@@ -565,7 +565,7 @@
       </c>
       <c r="E6" s="4">
         <f>_xll.qlPiecewiseYieldCurveDates(E3)</f>
-        <v>42675</v>
+        <v>42676</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -589,7 +589,7 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-47.516666666666666</v>
+        <v>-47.519444444444446</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -597,7 +597,7 @@
       </c>
       <c r="E8">
         <f>_xll.qlPiecewiseYieldCurveJumpTimes(E3)</f>
-        <v>-47.516666666666666</v>
+        <v>-47.519444444444446</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>